<commit_message>
Fix "Res multicodes" QC report formatting
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_report_town_close_res_multicodes.xlsx
+++ b/dbt/export/templates/qc.vw_report_town_close_res_multicodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACC6ED80-20FA-463E-BF5B-F066447ACEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66713ACB-CBB1-4E2A-9837-D5D1EC3DA461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33345" yWindow="3690" windowWidth="21600" windowHeight="11295" xr2:uid="{43356FB7-CF47-40B1-A061-F107645226C3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43356FB7-CF47-40B1-A061-F107645226C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>PARID</t>
   </si>
@@ -83,7 +83,13 @@
     <t>2024 Total MV</t>
   </si>
   <si>
-    <t>2032 LMV</t>
+    <t>TAXYR</t>
+  </si>
+  <si>
+    <t>TOWNSHIP</t>
+  </si>
+  <si>
+    <t>2023 LMV</t>
   </si>
 </sst>
 </file>
@@ -170,9 +176,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -493,88 +498,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BDCE18-6048-4E04-8941-9AEDD30B90BA}">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Q1"/>
-      <c r="R1"/>
-      <c r="S1"/>
-      <c r="T1"/>
-      <c r="U1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>